<commit_message>
cierre 17 jun 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/CREDITOS  4 CARNES   ZAVALETA   JUNIO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/CREDITOS  4 CARNES   ZAVALETA   JUNIO    2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES OCTUBRE  2021     " sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="91">
   <si>
     <t>REMISION</t>
   </si>
@@ -4184,8 +4184,8 @@
   </sheetPr>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4470,33 +4470,45 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
+      <c r="A14" s="12">
+        <v>44722</v>
+      </c>
       <c r="B14" s="13">
         <v>384</v>
       </c>
       <c r="C14" s="24"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="20"/>
+      <c r="D14" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="20">
+        <v>11919</v>
+      </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
       <c r="H14" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11919</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="12">
+        <v>44723</v>
+      </c>
       <c r="B15" s="13">
         <v>385</v>
       </c>
       <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="20"/>
+      <c r="D15" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="20">
+        <v>41552</v>
+      </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
       <c r="H15" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>41552</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -4919,7 +4931,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="39">
         <f>SUM(E4:E43)</f>
-        <v>172749</v>
+        <v>226220</v>
       </c>
       <c r="F44" s="39"/>
       <c r="G44" s="39">
@@ -4928,7 +4940,7 @@
       </c>
       <c r="H44" s="40">
         <f>SUM(H4:H43)</f>
-        <v>166146</v>
+        <v>219617</v>
       </c>
       <c r="I44" s="2"/>
     </row>
@@ -4972,7 +4984,7 @@
       <c r="D48" s="2"/>
       <c r="E48" s="167">
         <f>E44-G44</f>
-        <v>166146</v>
+        <v>219617</v>
       </c>
       <c r="F48" s="168"/>
       <c r="G48" s="169"/>
@@ -15651,7 +15663,7 @@
   </sheetPr>
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CIERRE 22 JUN 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/CREDITOS  4 CARNES   ZAVALETA   JUNIO    2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #06  JUNIO 2022/CREDITOS  4 CARNES   ZAVALETA   JUNIO    2022.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="6015" yWindow="330" windowWidth="13905" windowHeight="10920" firstSheet="9" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES OCTUBRE  2021     " sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="REMISIONES  MAYO   2022   " sheetId="14" r:id="rId8"/>
     <sheet name="DEPOSITOS   ODELPA   Y  NORMA L" sheetId="8" r:id="rId9"/>
     <sheet name="  REMISIONES   JUNIO  2022   " sheetId="5" r:id="rId10"/>
-    <sheet name="Hoja6" sheetId="17" r:id="rId11"/>
+    <sheet name="DEPOSITOS A NORMA LEDO  central" sheetId="17" r:id="rId11"/>
     <sheet name="Hoja2" sheetId="9" r:id="rId12"/>
     <sheet name="Hoja5" sheetId="10" r:id="rId13"/>
     <sheet name="Hoja4" sheetId="16" r:id="rId14"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="93">
   <si>
     <t>REMISION</t>
   </si>
@@ -443,6 +443,25 @@
   </si>
   <si>
     <t>GRACIELA LEDO</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">DEPOSITOS  ZAVALETA   A     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FF990033"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   Norma Ledo (central )</t>
+    </r>
+  </si>
+  <si>
+    <t>NORMA LEDO</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1019,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="192">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1388,6 +1407,27 @@
     <xf numFmtId="7" fontId="23" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1397,10 +1437,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF66FFFF"/>
       <color rgb="FFFF99CC"/>
       <color rgb="FFCC0099"/>
       <color rgb="FF0000FF"/>
-      <color rgb="FF66FFFF"/>
       <color rgb="FF00FF00"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FF990033"/>
@@ -1636,6 +1676,139 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector recto 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1095375" y="13487400"/>
+          <a:ext cx="7467600" cy="47625"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>974913</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>78440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>694765</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>11209</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Conector angular 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="2482942" y="9047911"/>
+          <a:ext cx="10191194" cy="6158752"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 17037"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>517351</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685799" y="9115425"/>
+          <a:ext cx="8146877" cy="10001250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4184,8 +4357,8 @@
   </sheetPr>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5167,13 +5340,965 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="114"/>
+    <col min="2" max="2" width="15.140625" style="114" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="114" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="114" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="114" customWidth="1"/>
+    <col min="6" max="9" width="11.42578125" style="114"/>
+    <col min="10" max="10" width="14.85546875" style="138" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="115" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="114" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="142"/>
+    <col min="14" max="15" width="11.42578125" style="114"/>
+    <col min="16" max="16" width="13.85546875" style="114" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" style="114"/>
+    <col min="18" max="18" width="17.42578125" style="114" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="11.42578125" style="114"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="177"/>
+      <c r="B1" s="178"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="178"/>
+      <c r="E1" s="178"/>
+      <c r="F1" s="178"/>
+      <c r="G1" s="178"/>
+      <c r="H1" s="178"/>
+      <c r="I1" s="178"/>
+      <c r="J1" s="178"/>
+      <c r="K1" s="178"/>
+      <c r="L1" s="178"/>
+    </row>
+    <row r="2" spans="1:19" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="190" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="191"/>
+      <c r="D2" s="191"/>
+      <c r="E2" s="191"/>
+      <c r="F2" s="157"/>
+      <c r="G2" s="157"/>
+      <c r="H2" s="157"/>
+      <c r="I2" s="157"/>
+      <c r="J2" s="157"/>
+      <c r="K2" s="157"/>
+      <c r="L2" s="157"/>
+      <c r="M2" s="181"/>
+      <c r="N2" s="183"/>
+      <c r="O2" s="184"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="185"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="121"/>
+    </row>
+    <row r="3" spans="1:19" ht="33.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="132" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="134" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="139" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="133" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="101"/>
+      <c r="J3" s="137"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="186"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="183"/>
+      <c r="O3" s="184"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="185"/>
+      <c r="R3" s="62"/>
+      <c r="S3" s="121"/>
+    </row>
+    <row r="4" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="130">
+        <v>44720</v>
+      </c>
+      <c r="C4" s="135">
+        <v>44722</v>
+      </c>
+      <c r="D4" s="131">
+        <v>45730</v>
+      </c>
+      <c r="E4" s="131">
+        <f>D4</f>
+        <v>45730</v>
+      </c>
+      <c r="I4" s="101"/>
+      <c r="J4" s="137"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="181"/>
+      <c r="N4" s="183"/>
+      <c r="O4" s="184"/>
+      <c r="P4" s="62"/>
+      <c r="Q4" s="185"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="121"/>
+    </row>
+    <row r="5" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="130">
+        <v>44721</v>
+      </c>
+      <c r="C5" s="136">
+        <v>44722</v>
+      </c>
+      <c r="D5" s="20">
+        <v>44700</v>
+      </c>
+      <c r="E5" s="20">
+        <f>E4+D5</f>
+        <v>90430</v>
+      </c>
+      <c r="I5" s="101"/>
+      <c r="J5" s="137"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="181"/>
+      <c r="N5" s="183"/>
+      <c r="O5" s="184"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="185"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="121"/>
+    </row>
+    <row r="6" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="130">
+        <v>44722</v>
+      </c>
+      <c r="C6" s="136">
+        <v>44725</v>
+      </c>
+      <c r="D6" s="20">
+        <v>45943</v>
+      </c>
+      <c r="E6" s="20">
+        <f>E5+D6</f>
+        <v>136373</v>
+      </c>
+      <c r="I6" s="101"/>
+      <c r="J6" s="137"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="181"/>
+      <c r="N6" s="183"/>
+      <c r="O6" s="184"/>
+      <c r="P6" s="62"/>
+      <c r="Q6" s="185"/>
+      <c r="R6" s="62"/>
+      <c r="S6" s="121"/>
+    </row>
+    <row r="7" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="130">
+        <v>44723</v>
+      </c>
+      <c r="C7" s="136">
+        <v>44725</v>
+      </c>
+      <c r="D7" s="20">
+        <v>16613.5</v>
+      </c>
+      <c r="E7" s="20">
+        <f t="shared" ref="E7:E22" si="0">E6+D7</f>
+        <v>152986.5</v>
+      </c>
+      <c r="I7" s="101"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="181"/>
+      <c r="N7" s="183"/>
+      <c r="O7" s="184"/>
+      <c r="P7" s="62"/>
+      <c r="Q7" s="185"/>
+      <c r="R7" s="62"/>
+      <c r="S7" s="121"/>
+    </row>
+    <row r="8" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="130">
+        <v>44724</v>
+      </c>
+      <c r="C8" s="136">
+        <v>44725</v>
+      </c>
+      <c r="D8" s="20">
+        <v>17154</v>
+      </c>
+      <c r="E8" s="20">
+        <f t="shared" si="0"/>
+        <v>170140.5</v>
+      </c>
+      <c r="I8" s="101"/>
+      <c r="J8" s="137"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="181"/>
+      <c r="N8" s="183"/>
+      <c r="O8" s="184"/>
+      <c r="P8" s="62"/>
+      <c r="Q8" s="185"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="121"/>
+    </row>
+    <row r="9" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="130">
+        <v>44725</v>
+      </c>
+      <c r="C9" s="136">
+        <v>44728</v>
+      </c>
+      <c r="D9" s="20">
+        <v>50350</v>
+      </c>
+      <c r="E9" s="20">
+        <f t="shared" si="0"/>
+        <v>220490.5</v>
+      </c>
+      <c r="I9" s="101"/>
+      <c r="J9" s="137"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="181"/>
+      <c r="N9" s="183"/>
+      <c r="O9" s="184"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="185"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="121"/>
+    </row>
+    <row r="10" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="130">
+        <v>44726</v>
+      </c>
+      <c r="C10" s="136">
+        <v>44728</v>
+      </c>
+      <c r="D10" s="20">
+        <v>44920</v>
+      </c>
+      <c r="E10" s="20">
+        <f t="shared" si="0"/>
+        <v>265410.5</v>
+      </c>
+      <c r="I10" s="101"/>
+      <c r="J10" s="137"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="181"/>
+      <c r="N10" s="183"/>
+      <c r="O10" s="184"/>
+      <c r="P10" s="62"/>
+      <c r="Q10" s="185"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="121"/>
+    </row>
+    <row r="11" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="130">
+        <v>44727</v>
+      </c>
+      <c r="C11" s="136">
+        <v>44728</v>
+      </c>
+      <c r="D11" s="20">
+        <v>36290.5</v>
+      </c>
+      <c r="E11" s="20">
+        <f t="shared" si="0"/>
+        <v>301701</v>
+      </c>
+      <c r="I11" s="101"/>
+      <c r="J11" s="137"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="181"/>
+      <c r="N11" s="183"/>
+      <c r="O11" s="184"/>
+      <c r="P11" s="62"/>
+      <c r="Q11" s="185"/>
+      <c r="R11" s="62"/>
+      <c r="S11" s="121"/>
+    </row>
+    <row r="12" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="130">
+        <v>44728</v>
+      </c>
+      <c r="C12" s="136">
+        <v>44732</v>
+      </c>
+      <c r="D12" s="20">
+        <v>49576</v>
+      </c>
+      <c r="E12" s="20">
+        <f t="shared" si="0"/>
+        <v>351277</v>
+      </c>
+      <c r="I12" s="101"/>
+      <c r="J12" s="137"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="181"/>
+      <c r="N12" s="183"/>
+      <c r="O12" s="184"/>
+      <c r="P12" s="62"/>
+      <c r="Q12" s="185"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="121"/>
+    </row>
+    <row r="13" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="130">
+        <v>44729</v>
+      </c>
+      <c r="C13" s="136">
+        <v>44732</v>
+      </c>
+      <c r="D13" s="22">
+        <v>48123</v>
+      </c>
+      <c r="E13" s="20">
+        <f t="shared" si="0"/>
+        <v>399400</v>
+      </c>
+      <c r="I13" s="101"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="181"/>
+      <c r="N13" s="183"/>
+      <c r="O13" s="184"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="185"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="121"/>
+    </row>
+    <row r="14" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="130">
+        <v>44730</v>
+      </c>
+      <c r="C14" s="136">
+        <v>44732</v>
+      </c>
+      <c r="D14" s="20">
+        <v>66300</v>
+      </c>
+      <c r="E14" s="20">
+        <f t="shared" si="0"/>
+        <v>465700</v>
+      </c>
+      <c r="I14" s="101"/>
+      <c r="J14" s="137"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="181"/>
+      <c r="N14" s="183"/>
+      <c r="O14" s="184"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="185"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="121"/>
+    </row>
+    <row r="15" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="130">
+        <v>44731</v>
+      </c>
+      <c r="C15" s="136">
+        <v>44732</v>
+      </c>
+      <c r="D15" s="20">
+        <v>75117</v>
+      </c>
+      <c r="E15" s="20">
+        <f t="shared" si="0"/>
+        <v>540817</v>
+      </c>
+      <c r="I15" s="101"/>
+      <c r="J15" s="137"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="181"/>
+      <c r="N15" s="183"/>
+      <c r="O15" s="184"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="185"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="121"/>
+    </row>
+    <row r="16" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="130"/>
+      <c r="C16" s="136"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20">
+        <f t="shared" si="0"/>
+        <v>540817</v>
+      </c>
+      <c r="I16" s="101"/>
+      <c r="J16" s="137"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="181"/>
+      <c r="N16" s="183"/>
+      <c r="O16" s="184"/>
+      <c r="P16" s="62"/>
+      <c r="Q16" s="185"/>
+      <c r="R16" s="62"/>
+      <c r="S16" s="121"/>
+    </row>
+    <row r="17" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="130"/>
+      <c r="C17" s="136"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20">
+        <f t="shared" si="0"/>
+        <v>540817</v>
+      </c>
+      <c r="I17" s="101"/>
+      <c r="J17" s="137"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="181"/>
+      <c r="N17" s="183"/>
+      <c r="O17" s="184"/>
+      <c r="P17" s="62"/>
+      <c r="Q17" s="185"/>
+      <c r="R17" s="62"/>
+      <c r="S17" s="121"/>
+    </row>
+    <row r="18" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="130"/>
+      <c r="C18" s="136"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20">
+        <f t="shared" si="0"/>
+        <v>540817</v>
+      </c>
+      <c r="I18" s="101"/>
+      <c r="J18" s="137"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="187"/>
+      <c r="M18" s="181"/>
+      <c r="N18" s="183"/>
+      <c r="O18" s="184"/>
+      <c r="P18" s="62"/>
+      <c r="Q18" s="185"/>
+      <c r="R18" s="62"/>
+      <c r="S18" s="121"/>
+    </row>
+    <row r="19" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="130"/>
+      <c r="C19" s="136"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20">
+        <f t="shared" si="0"/>
+        <v>540817</v>
+      </c>
+      <c r="I19" s="101"/>
+      <c r="J19" s="137"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="181"/>
+      <c r="N19" s="183"/>
+      <c r="O19" s="184"/>
+      <c r="P19" s="62"/>
+      <c r="Q19" s="185"/>
+      <c r="R19" s="62"/>
+      <c r="S19" s="121"/>
+    </row>
+    <row r="20" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+      <c r="A20" s="121"/>
+      <c r="B20" s="130"/>
+      <c r="C20" s="136"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20">
+        <f t="shared" si="0"/>
+        <v>540817</v>
+      </c>
+      <c r="F20" s="121"/>
+      <c r="G20" s="121"/>
+      <c r="H20" s="121"/>
+      <c r="I20" s="188"/>
+      <c r="J20" s="137"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="181"/>
+      <c r="N20" s="183"/>
+      <c r="O20" s="184"/>
+      <c r="P20" s="62"/>
+      <c r="Q20" s="185"/>
+      <c r="R20" s="62"/>
+      <c r="S20" s="121"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="121"/>
+      <c r="B21" s="130"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20">
+        <f t="shared" si="0"/>
+        <v>540817</v>
+      </c>
+      <c r="F21" s="121"/>
+      <c r="G21" s="121"/>
+      <c r="H21" s="121"/>
+      <c r="I21" s="101"/>
+      <c r="J21" s="137"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="181"/>
+      <c r="N21" s="183"/>
+      <c r="O21" s="184"/>
+      <c r="P21" s="62"/>
+      <c r="Q21" s="185"/>
+      <c r="R21" s="62"/>
+      <c r="S21" s="121"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="121"/>
+      <c r="B22" s="130"/>
+      <c r="C22" s="136"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="160">
+        <f t="shared" si="0"/>
+        <v>540817</v>
+      </c>
+      <c r="F22" s="121"/>
+      <c r="G22" s="121"/>
+      <c r="H22" s="121"/>
+      <c r="I22" s="101"/>
+      <c r="J22" s="137"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="181"/>
+      <c r="N22" s="183"/>
+      <c r="O22" s="184"/>
+      <c r="P22" s="62"/>
+      <c r="Q22" s="185"/>
+      <c r="R22" s="62"/>
+      <c r="S22" s="129"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="121"/>
+      <c r="B23" s="130"/>
+      <c r="C23" s="136"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="121"/>
+      <c r="G23" s="121"/>
+      <c r="H23" s="121"/>
+      <c r="I23" s="101"/>
+      <c r="J23" s="137"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="181"/>
+      <c r="N23" s="121"/>
+      <c r="O23" s="121"/>
+      <c r="P23" s="121"/>
+      <c r="Q23" s="121"/>
+      <c r="R23" s="189"/>
+      <c r="S23" s="121"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="121"/>
+      <c r="B24" s="130"/>
+      <c r="C24" s="136"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="121"/>
+      <c r="G24" s="121"/>
+      <c r="H24" s="121"/>
+      <c r="I24" s="101"/>
+      <c r="J24" s="137"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="181"/>
+      <c r="N24" s="121"/>
+      <c r="O24" s="121"/>
+      <c r="P24" s="121"/>
+      <c r="Q24" s="121"/>
+      <c r="R24" s="121"/>
+      <c r="S24" s="121"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="121"/>
+      <c r="B25" s="130"/>
+      <c r="C25" s="136"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="22">
+        <v>850487.81</v>
+      </c>
+      <c r="F25" s="121"/>
+      <c r="G25" s="121"/>
+      <c r="H25" s="121"/>
+      <c r="I25" s="101"/>
+      <c r="J25" s="137"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+    </row>
+    <row r="26" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+      <c r="B26" s="157"/>
+      <c r="C26" s="157"/>
+      <c r="D26" s="157"/>
+      <c r="E26" s="157"/>
+      <c r="F26" s="157"/>
+      <c r="G26" s="157"/>
+      <c r="H26" s="157"/>
+      <c r="I26" s="157"/>
+      <c r="J26" s="157"/>
+      <c r="K26" s="157"/>
+      <c r="L26" s="157"/>
+    </row>
+    <row r="28" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K39" s="162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K40" s="163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K41" s="163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K42" s="163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="121"/>
+      <c r="B43" s="121"/>
+      <c r="C43" s="121"/>
+      <c r="D43" s="121"/>
+      <c r="E43" s="121"/>
+      <c r="F43" s="121"/>
+      <c r="G43" s="121"/>
+      <c r="H43" s="121"/>
+      <c r="K43" s="163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="121"/>
+      <c r="B44" s="121"/>
+      <c r="C44" s="121"/>
+      <c r="D44" s="121"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="121"/>
+      <c r="G44" s="121"/>
+      <c r="H44" s="121"/>
+      <c r="I44" s="101"/>
+      <c r="J44" s="137"/>
+      <c r="K44" s="163">
+        <v>0</v>
+      </c>
+      <c r="L44" s="60"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="121"/>
+      <c r="B45" s="121"/>
+      <c r="C45" s="121"/>
+      <c r="D45" s="121"/>
+      <c r="E45" s="121"/>
+      <c r="F45" s="121"/>
+      <c r="G45" s="121"/>
+      <c r="H45" s="121"/>
+      <c r="I45" s="101"/>
+      <c r="J45" s="137"/>
+      <c r="K45" s="163">
+        <v>0</v>
+      </c>
+      <c r="L45" s="60"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="121"/>
+      <c r="B46" s="121"/>
+      <c r="C46" s="121"/>
+      <c r="D46" s="121"/>
+      <c r="E46" s="121"/>
+      <c r="F46" s="121"/>
+      <c r="G46" s="121"/>
+      <c r="H46" s="121"/>
+      <c r="I46" s="101"/>
+      <c r="J46" s="137"/>
+      <c r="K46" s="163">
+        <v>0</v>
+      </c>
+      <c r="L46" s="60"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="121"/>
+      <c r="B47" s="121"/>
+      <c r="C47" s="121"/>
+      <c r="D47" s="121"/>
+      <c r="E47" s="121"/>
+      <c r="F47" s="121"/>
+      <c r="G47" s="121"/>
+      <c r="H47" s="121"/>
+      <c r="I47" s="101"/>
+      <c r="J47" s="137"/>
+      <c r="K47" s="163">
+        <v>0</v>
+      </c>
+      <c r="L47" s="60"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="121"/>
+      <c r="B48" s="121"/>
+      <c r="C48" s="121"/>
+      <c r="D48" s="121"/>
+      <c r="E48" s="121"/>
+      <c r="F48" s="121"/>
+      <c r="G48" s="121"/>
+      <c r="H48" s="121"/>
+      <c r="I48" s="101"/>
+      <c r="J48" s="137"/>
+      <c r="K48" s="163">
+        <v>0</v>
+      </c>
+      <c r="L48" s="60"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="121"/>
+      <c r="B49" s="121"/>
+      <c r="C49" s="121"/>
+      <c r="D49" s="121"/>
+      <c r="E49" s="121"/>
+      <c r="F49" s="121"/>
+      <c r="G49" s="121"/>
+      <c r="H49" s="121"/>
+      <c r="I49" s="101"/>
+      <c r="J49" s="137"/>
+      <c r="K49" s="163">
+        <v>0</v>
+      </c>
+      <c r="L49" s="60"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A50" s="121"/>
+      <c r="B50" s="121"/>
+      <c r="C50" s="121"/>
+      <c r="D50" s="121"/>
+      <c r="E50" s="121"/>
+      <c r="F50" s="121"/>
+      <c r="G50" s="121"/>
+      <c r="H50" s="121"/>
+      <c r="I50" s="101"/>
+      <c r="J50" s="137"/>
+      <c r="K50" s="163">
+        <v>0</v>
+      </c>
+      <c r="L50" s="60"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A51" s="121"/>
+      <c r="B51" s="121"/>
+      <c r="C51" s="121"/>
+      <c r="D51" s="121"/>
+      <c r="E51" s="121"/>
+      <c r="F51" s="121"/>
+      <c r="G51" s="121"/>
+      <c r="H51" s="121"/>
+      <c r="I51" s="101"/>
+      <c r="J51" s="137"/>
+      <c r="K51" s="163">
+        <v>0</v>
+      </c>
+      <c r="L51" s="60"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A52" s="121"/>
+      <c r="B52" s="121"/>
+      <c r="C52" s="121"/>
+      <c r="D52" s="121"/>
+      <c r="E52" s="121"/>
+      <c r="F52" s="121"/>
+      <c r="G52" s="121"/>
+      <c r="H52" s="121"/>
+      <c r="I52" s="101"/>
+      <c r="J52" s="137"/>
+      <c r="K52" s="163">
+        <v>0</v>
+      </c>
+      <c r="L52" s="60"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="121"/>
+      <c r="B53" s="121"/>
+      <c r="C53" s="121"/>
+      <c r="D53" s="121"/>
+      <c r="E53" s="121"/>
+      <c r="F53" s="121"/>
+      <c r="G53" s="121"/>
+      <c r="H53" s="121"/>
+      <c r="I53" s="101"/>
+      <c r="J53" s="137"/>
+      <c r="K53" s="163">
+        <v>0</v>
+      </c>
+      <c r="L53" s="60"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="121"/>
+      <c r="B54" s="121"/>
+      <c r="C54" s="121"/>
+      <c r="D54" s="121"/>
+      <c r="E54" s="121"/>
+      <c r="F54" s="121"/>
+      <c r="G54" s="121"/>
+      <c r="H54" s="121"/>
+      <c r="I54" s="101"/>
+      <c r="J54" s="137"/>
+      <c r="K54" s="163">
+        <v>0</v>
+      </c>
+      <c r="L54" s="60"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="121"/>
+      <c r="B55" s="121"/>
+      <c r="C55" s="121"/>
+      <c r="D55" s="121"/>
+      <c r="E55" s="121"/>
+      <c r="F55" s="121"/>
+      <c r="G55" s="121"/>
+      <c r="H55" s="121"/>
+      <c r="I55" s="101"/>
+      <c r="J55" s="137"/>
+      <c r="K55" s="163">
+        <v>0</v>
+      </c>
+      <c r="L55" s="60"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56" s="121"/>
+      <c r="B56" s="121"/>
+      <c r="C56" s="121"/>
+      <c r="D56" s="121"/>
+      <c r="E56" s="121"/>
+      <c r="F56" s="121"/>
+      <c r="G56" s="121"/>
+      <c r="H56" s="121"/>
+      <c r="I56" s="101"/>
+      <c r="J56" s="137"/>
+      <c r="K56" s="163">
+        <v>0</v>
+      </c>
+      <c r="L56" s="60"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A57" s="121"/>
+      <c r="B57" s="121"/>
+      <c r="C57" s="121"/>
+      <c r="D57" s="121"/>
+      <c r="E57" s="121"/>
+      <c r="F57" s="121"/>
+      <c r="G57" s="121"/>
+      <c r="H57" s="121"/>
+      <c r="I57" s="101"/>
+      <c r="J57" s="137"/>
+      <c r="K57" s="163">
+        <v>0</v>
+      </c>
+      <c r="L57" s="60"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A58" s="121"/>
+      <c r="B58" s="121"/>
+      <c r="C58" s="121"/>
+      <c r="D58" s="121"/>
+      <c r="E58" s="121"/>
+      <c r="F58" s="121"/>
+      <c r="G58" s="121"/>
+      <c r="H58" s="121"/>
+      <c r="I58" s="101"/>
+      <c r="J58" s="137"/>
+      <c r="K58" s="163">
+        <v>0</v>
+      </c>
+      <c r="L58" s="60"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A59" s="121"/>
+      <c r="B59" s="121"/>
+      <c r="C59" s="121"/>
+      <c r="D59" s="121"/>
+      <c r="E59" s="121"/>
+      <c r="F59" s="121"/>
+      <c r="G59" s="121"/>
+      <c r="H59" s="121"/>
+      <c r="I59" s="101"/>
+      <c r="J59" s="137"/>
+      <c r="K59" s="163">
+        <v>0</v>
+      </c>
+      <c r="L59" s="60"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K60" s="163">
+        <v>0</v>
+      </c>
+      <c r="L60" s="60"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K61" s="163">
+        <v>0</v>
+      </c>
+      <c r="L61" s="129"/>
+    </row>
+    <row r="62" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K62" s="162">
+        <v>0</v>
+      </c>
+      <c r="L62" s="121"/>
+    </row>
+    <row r="63" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K63" s="179">
+        <f>SUM(K39:K62)</f>
+        <v>0</v>
+      </c>
+      <c r="L63" s="180"/>
+    </row>
+    <row r="68" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K68" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="K63:L63"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15663,8 +16788,8 @@
   </sheetPr>
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>